<commit_message>
asi si se hacian las fichas
</commit_message>
<xml_diff>
--- a/HT-4/Optica BAC-03-Ficha tecnica de un canal.xlsx
+++ b/HT-4/Optica BAC-03-Ficha tecnica de un canal.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/juan/Documents/Universidad/2022-20/arquiemp/repo/arquiemp/HT-4/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{492FCA9A-BDDF-A84A-B984-E8B4FDE09FE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33A93CA4-A7D8-D84A-BADF-954F5817932D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="-5900" windowWidth="38400" windowHeight="21100" xr2:uid="{6D2ADF59-F33A-44E3-88FB-8431094B32CC}"/>
+    <workbookView xWindow="28800" yWindow="-5900" windowWidth="38400" windowHeight="21100" activeTab="6" xr2:uid="{6D2ADF59-F33A-44E3-88FB-8431094B32CC}"/>
   </bookViews>
   <sheets>
     <sheet name="BAC-03-1" sheetId="1" r:id="rId1"/>
@@ -19,10 +19,9 @@
     <sheet name="BAC-03-4" sheetId="9" r:id="rId4"/>
     <sheet name="BAC-03-5" sheetId="10" r:id="rId5"/>
     <sheet name="BAC-03-6" sheetId="11" r:id="rId6"/>
-    <sheet name="BAC-03-7" sheetId="12" r:id="rId7"/>
-    <sheet name="BAC-03-8" sheetId="13" r:id="rId8"/>
-    <sheet name="BAC-03-9" sheetId="14" r:id="rId9"/>
-    <sheet name="BAC-03-10" sheetId="15" r:id="rId10"/>
+    <sheet name="BAC-03-7" sheetId="13" r:id="rId7"/>
+    <sheet name="BAC-03-8" sheetId="14" r:id="rId8"/>
+    <sheet name="BAC-03-10" sheetId="15" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -43,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="64">
   <si>
     <t>Nombre</t>
   </si>
@@ -96,9 +95,6 @@
     <t>R4</t>
   </si>
   <si>
-    <t>Exámen Visual</t>
-  </si>
-  <si>
     <t>D1</t>
   </si>
   <si>
@@ -111,24 +107,12 @@
     <t>M1</t>
   </si>
   <si>
-    <t>Pago en efectivo</t>
-  </si>
-  <si>
     <t>Monetización</t>
   </si>
   <si>
-    <t>M2</t>
-  </si>
-  <si>
-    <t>Pago con tarjeta</t>
-  </si>
-  <si>
     <t>A1</t>
   </si>
   <si>
-    <t>Aprovisioinamiento de monturas</t>
-  </si>
-  <si>
     <t>Aprovisioinamiento</t>
   </si>
   <si>
@@ -150,100 +134,106 @@
     <t>Transformación</t>
   </si>
   <si>
-    <t>Revisar la fórmula a aplicar</t>
-  </si>
-  <si>
     <t>Defiinir el tipo de corte que se la hará al lente</t>
   </si>
   <si>
-    <t>Cortar el lente de acuerdo con lo definido</t>
-  </si>
-  <si>
     <t>Pulir el lente</t>
   </si>
   <si>
     <t>Cliente</t>
   </si>
   <si>
-    <t>Montura</t>
-  </si>
-  <si>
     <t>-</t>
   </si>
   <si>
-    <t>El cliente escoge una montura</t>
-  </si>
-  <si>
-    <t>El cliente pregunta por el precio de la montura</t>
-  </si>
-  <si>
-    <t>Se genera una orden de compra por la montura</t>
-  </si>
-  <si>
-    <t>El cliente llega a la óptica</t>
-  </si>
-  <si>
-    <t>El cliente pregunta por la fabricación de unos lentes con su fórmula</t>
-  </si>
-  <si>
-    <t>Se le pide la fórmula al cliente</t>
-  </si>
-  <si>
-    <t>Se le da la cotización de los lentes al cliente</t>
-  </si>
-  <si>
-    <t>El cliente acepta o no el pago</t>
-  </si>
-  <si>
-    <t>De aceptar se genera una orden de compra para los lentes con dichas especificaciones</t>
-  </si>
-  <si>
-    <t>Se le entregan los lentes al cliente</t>
-  </si>
-  <si>
-    <t>Se arreglan las gafas del cliente</t>
-  </si>
-  <si>
-    <t>Se le devuelven las gafas al cliente</t>
-  </si>
-  <si>
-    <t>El cliente observa las monturas en el mostrador</t>
-  </si>
-  <si>
-    <t>Se le entrega la montura al cliente, con lentes sin fórmula</t>
-  </si>
-  <si>
     <t>Cliente, empleado</t>
   </si>
   <si>
     <t>Empleado</t>
   </si>
   <si>
-    <t>Se le pide al cliente una montura, sea una de su propiedad o una disponible en la tienda.</t>
-  </si>
-  <si>
     <t>Empleado, cliente</t>
   </si>
   <si>
-    <t>Lentes y/o montura</t>
-  </si>
-  <si>
-    <t>Pregunta al empleado si es posible arreglar las monturas</t>
-  </si>
-  <si>
-    <t>El empleado hace la cotización de la reparación</t>
-  </si>
-  <si>
-    <t>El empleado genera la orden de pago por el arreglo</t>
-  </si>
-  <si>
-    <t>Empleado - cliente</t>
-  </si>
-  <si>
-    <t>El cliente entrega las monturas con los lentes al empleado</t>
-  </si>
-  <si>
-    <t>Monturas a arreglar, lentes a arreglar</t>
+    <t>Examen Visual</t>
+  </si>
+  <si>
+    <t>Cliente, optómetra</t>
+  </si>
+  <si>
+    <t>Consultorio</t>
+  </si>
+  <si>
+    <t>Laboratorio</t>
+  </si>
+  <si>
+    <t>Caja registradora, datáfono</t>
+  </si>
+  <si>
+    <t>Sistema informático</t>
+  </si>
+  <si>
+    <t>Permitirle al cliente observar las monturas en el mostrador</t>
+  </si>
+  <si>
+    <t>Permitirle al cliente escoge una o varias monturas</t>
+  </si>
+  <si>
+    <t>Permitirle al cliente preguntar por el precio de la(s) montura(s)</t>
+  </si>
+  <si>
+    <t>Se le permite al cliente preguntar por el costo de fabricación de unos lentes con una formulacion determinada o con unas especificaciones determinadas (lentes de sol, lentes transition, etc)</t>
+  </si>
+  <si>
+    <t>Se le permite al cliente cotizar el tipo de lentes que desea, y si es necesaria una fórmula médica o no, o si desea comprarlos junto con una montura o tiene una de su propiedad.</t>
+  </si>
+  <si>
+    <t>Se le permite al cliente preguntar es posible arreglar sus monturas</t>
+  </si>
+  <si>
+    <t>Se le entrega al cliente una cotización de la reparación</t>
+  </si>
+  <si>
+    <t>Realizar el arreglo respectivo de las monturas</t>
+  </si>
+  <si>
+    <t>Se le permite al cliente realizarse un exámen visual dentro de un consultorio en la óptica</t>
+  </si>
+  <si>
+    <t>Se le entrega al cliente una formulación médica avalada. La fórmula contiene el aumento de los lentes y posiblemente algunos medicamentos.</t>
+  </si>
+  <si>
+    <t>Notificar al cliente de que su producto está listo para ser recogido mediante un mensaje de texto al celular</t>
+  </si>
+  <si>
+    <t>Entregarle al cliente el producto dentro de la óptica</t>
+  </si>
+  <si>
+    <t>Cobro a los compradores</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reembolsar al comprador el pago de un producto devuelto </t>
+  </si>
+  <si>
+    <t>Permite al empleado hacer el pago de los productos comprados, ya sea con una tarjeta o en efectivo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hacer pedidos, recibir los pedidos y almacenarlos en las bodegas, recibir las facturas y hacer los pagos respectivos </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Manejar devoluciones, reclamos y procesos de aseguramiento de calidad con los proveedores </t>
+  </si>
+  <si>
+    <t>Cortar el lente de acuerdo con la montura definida</t>
+  </si>
+  <si>
+    <t>Revisar la fórmula o las modificaciones a aplicar</t>
+  </si>
+  <si>
+    <t>Empleado laboratorio</t>
+  </si>
+  <si>
+    <t>Aprovisioinamiento de lentes</t>
   </si>
 </sst>
 </file>
@@ -291,7 +281,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -314,11 +304,33 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -341,12 +353,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -663,8 +683,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4ABDEE2F-9DA5-4F4F-A9BF-B9BEA22ACD0E}">
   <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView showGridLines="0" zoomScale="150" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -734,89 +754,65 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="15" x14ac:dyDescent="0.15">
-      <c r="A10" s="6">
+    <row r="10" spans="1:4" ht="30" x14ac:dyDescent="0.15">
+      <c r="A10" s="8">
         <v>1</v>
       </c>
       <c r="B10" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.15">
+      <c r="A11" s="6">
+        <v>2</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="45" x14ac:dyDescent="0.15">
+      <c r="A12" s="11">
+        <v>3</v>
+      </c>
+      <c r="B12" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="C10" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.15">
-      <c r="A11" s="8">
-        <v>2</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="C11" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="D11" s="8" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="15" x14ac:dyDescent="0.15">
-      <c r="A12" s="6">
-        <v>3</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="D12" s="6" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.15">
-      <c r="A13" s="6">
-        <v>4</v>
-      </c>
-      <c r="B13" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="D13" s="6" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="30" x14ac:dyDescent="0.15">
-      <c r="A14" s="6">
-        <v>5</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="C14" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="D14" s="6" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="30" x14ac:dyDescent="0.15">
-      <c r="A15" s="6">
-        <v>6</v>
-      </c>
-      <c r="B15" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="C15" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="D15" s="6" t="s">
-        <v>40</v>
-      </c>
+      <c r="C12" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="D12" s="11" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A13" s="12"/>
+      <c r="B13" s="12"/>
+      <c r="C13" s="12"/>
+      <c r="D13" s="12"/>
+    </row>
+    <row r="14" spans="1:4" s="15" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A14" s="14"/>
+      <c r="B14" s="14"/>
+      <c r="C14" s="14"/>
+      <c r="D14" s="14"/>
+    </row>
+    <row r="15" spans="1:4" s="15" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A15" s="14"/>
+      <c r="B15" s="14"/>
+      <c r="C15" s="14"/>
+      <c r="D15" s="14"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A16" s="9"/>
@@ -829,153 +825,6 @@
       <c r="B17" s="9"/>
       <c r="C17" s="9"/>
       <c r="D17" s="9"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6F2B678-6A08-4DCD-A7B0-10E20E2DA48D}">
-  <dimension ref="A1:D17"/>
-  <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
-  <cols>
-    <col min="1" max="1" width="8.33203125" customWidth="1"/>
-    <col min="2" max="2" width="27" customWidth="1"/>
-    <col min="3" max="4" width="16" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A4" s="1"/>
-    </row>
-    <row r="5" spans="1:4" ht="15" x14ac:dyDescent="0.15">
-      <c r="A5" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="15" x14ac:dyDescent="0.15">
-      <c r="A6" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="C6" s="2"/>
-    </row>
-    <row r="7" spans="1:4" ht="15" x14ac:dyDescent="0.15">
-      <c r="A7" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A8" s="1"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A9" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="15" x14ac:dyDescent="0.15">
-      <c r="A10" s="7">
-        <v>1</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
-    </row>
-    <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.15">
-      <c r="A11" s="7">
-        <v>2</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
-    </row>
-    <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.15">
-      <c r="A12" s="7">
-        <v>3</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
-    </row>
-    <row r="13" spans="1:4" ht="15" x14ac:dyDescent="0.15">
-      <c r="A13" s="7">
-        <v>4</v>
-      </c>
-      <c r="B13" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="C13" s="6"/>
-      <c r="D13" s="6"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A14" s="7">
-        <v>5</v>
-      </c>
-      <c r="B14" s="6"/>
-      <c r="C14" s="6"/>
-      <c r="D14" s="6"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A15" s="6"/>
-      <c r="B15" s="6"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A16" s="6"/>
-      <c r="B16" s="6"/>
-      <c r="C16" s="6"/>
-      <c r="D16" s="6"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A17" s="6"/>
-      <c r="B17" s="6"/>
-      <c r="C17" s="6"/>
-      <c r="D17" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -985,10 +834,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{692DA9A4-5D1E-40C9-8FE0-6DBF8AAC097A}">
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="125" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -1059,122 +908,49 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="15" x14ac:dyDescent="0.15">
-      <c r="A10" s="6">
+    <row r="10" spans="1:4" ht="105" x14ac:dyDescent="0.15">
+      <c r="A10" s="8">
         <v>1</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="45" x14ac:dyDescent="0.15">
-      <c r="A11" s="8">
+        <v>46</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="105" x14ac:dyDescent="0.15">
+      <c r="A11" s="6">
         <v>2</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="C11" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="D11" s="8" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.15">
-      <c r="A12" s="6">
-        <v>3</v>
-      </c>
-      <c r="B12" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="C12" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="D12" s="6" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="60" x14ac:dyDescent="0.15">
-      <c r="A13" s="6">
-        <v>4</v>
-      </c>
-      <c r="B13" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="D13" s="6"/>
-    </row>
-    <row r="14" spans="1:4" ht="30" x14ac:dyDescent="0.15">
-      <c r="A14" s="6">
-        <v>5</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="C14" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="D14" s="6" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="15" x14ac:dyDescent="0.15">
-      <c r="A15" s="8">
-        <v>6</v>
-      </c>
-      <c r="B15" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="C15" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="D15" s="6" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="60" x14ac:dyDescent="0.15">
-      <c r="A16" s="6">
-        <v>7</v>
-      </c>
-      <c r="B16" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="C16" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="D16" s="10" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="30" x14ac:dyDescent="0.15">
-      <c r="A17" s="6">
-        <v>8</v>
-      </c>
-      <c r="B17" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="C17" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="D17" s="6" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A18" s="9"/>
-      <c r="B18" s="9"/>
-      <c r="C18" s="9"/>
-      <c r="D18" s="9"/>
-    </row>
+      <c r="C11" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" s="15" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A12" s="12"/>
+      <c r="B12" s="12"/>
+      <c r="C12" s="12"/>
+      <c r="D12" s="12"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A13" s="9"/>
+      <c r="B13" s="9"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="9"/>
+    </row>
+    <row r="17" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="18" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="19" customFormat="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -1183,10 +959,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E8F74C6-CDB7-4BA9-9E9D-400DD2814AFA}">
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="141" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -1256,18 +1032,18 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:4" ht="45" x14ac:dyDescent="0.15">
       <c r="A10" s="6">
         <v>1</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.15">
@@ -1275,13 +1051,13 @@
         <v>2</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>56</v>
+        <v>36</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.15">
@@ -1289,82 +1065,26 @@
         <v>3</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>59</v>
+        <v>36</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.15">
-      <c r="A13" s="6">
-        <v>4</v>
-      </c>
-      <c r="B13" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="D13" s="6" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="45" x14ac:dyDescent="0.15">
-      <c r="A14" s="6">
-        <v>5</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="C14" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="D14" s="6" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="30" x14ac:dyDescent="0.15">
-      <c r="A15" s="6">
-        <v>6</v>
-      </c>
-      <c r="B15" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="C15" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="D15" s="6" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="30" x14ac:dyDescent="0.15">
-      <c r="A16" s="6">
-        <v>7</v>
-      </c>
-      <c r="B16" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="C16" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="D16" s="6" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A17" s="9"/>
-      <c r="B17" s="9"/>
-      <c r="C17" s="9"/>
-      <c r="D17" s="9"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A18" s="9"/>
-      <c r="B18" s="9"/>
-      <c r="C18" s="9"/>
-      <c r="D18" s="9"/>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A13" s="9"/>
+      <c r="B13" s="9"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="9"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A14" s="9"/>
+      <c r="B14" s="9"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1374,10 +1094,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A38F5645-0415-42ED-9D08-03651B71959E}">
-  <dimension ref="A1:D17"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView showGridLines="0" zoomScale="166" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -1418,7 +1138,7 @@
         <v>0</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>17</v>
+        <v>37</v>
       </c>
       <c r="C6" s="2"/>
     </row>
@@ -1447,63 +1167,51 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:4" ht="60" x14ac:dyDescent="0.15">
       <c r="A10" s="6">
-        <v>1</v>
-      </c>
-      <c r="B10" s="6"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.15">
+        <v>2</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="75" x14ac:dyDescent="0.15">
       <c r="A11" s="6">
-        <v>2</v>
-      </c>
-      <c r="B11" s="6"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
+        <v>5</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A12" s="6">
-        <v>3</v>
-      </c>
-      <c r="B12" s="6"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
+      <c r="A12" s="12"/>
+      <c r="B12" s="12"/>
+      <c r="C12" s="12"/>
+      <c r="D12" s="12"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A13" s="6">
-        <v>4</v>
-      </c>
-      <c r="B13" s="6"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="6"/>
+      <c r="A13" s="14"/>
+      <c r="B13" s="14"/>
+      <c r="C13" s="14"/>
+      <c r="D13" s="14"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A14" s="6">
-        <v>5</v>
-      </c>
-      <c r="B14" s="6"/>
-      <c r="C14" s="6"/>
-      <c r="D14" s="6"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A15" s="6"/>
-      <c r="B15" s="6"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A16" s="6"/>
-      <c r="B16" s="6"/>
-      <c r="C16" s="6"/>
-      <c r="D16" s="6"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A17" s="6"/>
-      <c r="B17" s="6"/>
-      <c r="C17" s="6"/>
-      <c r="D17" s="6"/>
+      <c r="A14" s="14"/>
+      <c r="B14" s="14"/>
+      <c r="C14" s="14"/>
+      <c r="D14" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1513,10 +1221,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E140821C-16ED-41F3-BBD2-5EE5717C381F}">
-  <dimension ref="A1:D17"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView showGridLines="0" zoomScale="150" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -1549,7 +1257,7 @@
         <v>1</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="15" x14ac:dyDescent="0.15">
@@ -1557,7 +1265,7 @@
         <v>0</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C6" s="2"/>
     </row>
@@ -1566,7 +1274,7 @@
         <v>4</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -1586,63 +1294,51 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:4" ht="60" x14ac:dyDescent="0.15">
       <c r="A10" s="6">
         <v>1</v>
       </c>
-      <c r="B10" s="6"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="B10" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.15">
       <c r="A11" s="6">
         <v>2</v>
       </c>
-      <c r="B11" s="6"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
+      <c r="B11" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A12" s="6">
-        <v>3</v>
-      </c>
-      <c r="B12" s="6"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
+      <c r="A12" s="12"/>
+      <c r="B12" s="12"/>
+      <c r="C12" s="12"/>
+      <c r="D12" s="12"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A13" s="6">
-        <v>4</v>
-      </c>
-      <c r="B13" s="6"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="6"/>
+      <c r="A13" s="14"/>
+      <c r="B13" s="14"/>
+      <c r="C13" s="14"/>
+      <c r="D13" s="14"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A14" s="6">
-        <v>5</v>
-      </c>
-      <c r="B14" s="6"/>
-      <c r="C14" s="6"/>
-      <c r="D14" s="6"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A15" s="6"/>
-      <c r="B15" s="6"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A16" s="6"/>
-      <c r="B16" s="6"/>
-      <c r="C16" s="6"/>
-      <c r="D16" s="6"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A17" s="6"/>
-      <c r="B17" s="6"/>
-      <c r="C17" s="6"/>
-      <c r="D17" s="6"/>
+      <c r="A14" s="14"/>
+      <c r="B14" s="14"/>
+      <c r="C14" s="14"/>
+      <c r="D14" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1655,7 +1351,7 @@
   <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -1688,7 +1384,7 @@
         <v>1</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="15" x14ac:dyDescent="0.15">
@@ -1696,7 +1392,7 @@
         <v>0</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>22</v>
+        <v>55</v>
       </c>
       <c r="C6" s="2"/>
     </row>
@@ -1705,7 +1401,7 @@
         <v>4</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -1725,63 +1421,69 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:4" ht="60" x14ac:dyDescent="0.15">
       <c r="A10" s="6">
         <v>1</v>
       </c>
-      <c r="B10" s="6"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="B10" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="45" x14ac:dyDescent="0.15">
       <c r="A11" s="6">
         <v>2</v>
       </c>
-      <c r="B11" s="6"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
+      <c r="B11" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A12" s="6">
-        <v>3</v>
-      </c>
-      <c r="B12" s="6"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
+      <c r="A12" s="12"/>
+      <c r="B12" s="12"/>
+      <c r="C12" s="12"/>
+      <c r="D12" s="12"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A13" s="6">
-        <v>4</v>
-      </c>
-      <c r="B13" s="6"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="6"/>
+      <c r="A13" s="14"/>
+      <c r="B13" s="14"/>
+      <c r="C13" s="14"/>
+      <c r="D13" s="14"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A14" s="6">
-        <v>5</v>
-      </c>
-      <c r="B14" s="6"/>
-      <c r="C14" s="6"/>
-      <c r="D14" s="6"/>
+      <c r="A14" s="14"/>
+      <c r="B14" s="14"/>
+      <c r="C14" s="14"/>
+      <c r="D14" s="14"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A15" s="6"/>
-      <c r="B15" s="6"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
+      <c r="A15" s="14"/>
+      <c r="B15" s="14"/>
+      <c r="C15" s="14"/>
+      <c r="D15" s="14"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A16" s="6"/>
-      <c r="B16" s="6"/>
-      <c r="C16" s="6"/>
-      <c r="D16" s="6"/>
+      <c r="A16" s="14"/>
+      <c r="B16" s="14"/>
+      <c r="C16" s="14"/>
+      <c r="D16" s="14"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A17" s="6"/>
-      <c r="B17" s="6"/>
-      <c r="C17" s="6"/>
-      <c r="D17" s="6"/>
+      <c r="A17" s="14"/>
+      <c r="B17" s="14"/>
+      <c r="C17" s="14"/>
+      <c r="D17" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1790,11 +1492,11 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A729007-E66E-416B-8D9B-1411A3B40E8F}">
-  <dimension ref="A1:D17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BAD743F-5732-48A8-9B15-61A983AA847C}">
+  <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -1827,7 +1529,7 @@
         <v>1</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="15" x14ac:dyDescent="0.15">
@@ -1835,7 +1537,7 @@
         <v>0</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>25</v>
+        <v>63</v>
       </c>
       <c r="C6" s="2"/>
     </row>
@@ -1864,63 +1566,33 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:4" ht="60" x14ac:dyDescent="0.15">
       <c r="A10" s="6">
         <v>1</v>
       </c>
-      <c r="B10" s="6"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="B10" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="60" x14ac:dyDescent="0.15">
       <c r="A11" s="6">
         <v>2</v>
       </c>
-      <c r="B11" s="6"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A12" s="6">
-        <v>3</v>
-      </c>
-      <c r="B12" s="6"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A13" s="6">
-        <v>4</v>
-      </c>
-      <c r="B13" s="6"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="6"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A14" s="6">
-        <v>5</v>
-      </c>
-      <c r="B14" s="6"/>
-      <c r="C14" s="6"/>
-      <c r="D14" s="6"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A15" s="6"/>
-      <c r="B15" s="6"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A16" s="6"/>
-      <c r="B16" s="6"/>
-      <c r="C16" s="6"/>
-      <c r="D16" s="6"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A17" s="6"/>
-      <c r="B17" s="6"/>
-      <c r="C17" s="6"/>
-      <c r="D17" s="6"/>
+      <c r="B11" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>42</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1929,11 +1601,11 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BAD743F-5732-48A8-9B15-61A983AA847C}">
-  <dimension ref="A1:D17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D01BD858-72F0-4803-BCED-49D604DC8C85}">
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="D11" sqref="A10:D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -1966,15 +1638,15 @@
         <v>1</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.15">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C6" s="2"/>
     </row>
@@ -1983,7 +1655,7 @@
         <v>4</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -2003,63 +1675,33 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:4" ht="60" x14ac:dyDescent="0.15">
       <c r="A10" s="6">
         <v>1</v>
       </c>
-      <c r="B10" s="6"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="B10" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="60" x14ac:dyDescent="0.15">
       <c r="A11" s="6">
         <v>2</v>
       </c>
-      <c r="B11" s="6"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A12" s="6">
-        <v>3</v>
-      </c>
-      <c r="B12" s="6"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A13" s="6">
-        <v>4</v>
-      </c>
-      <c r="B13" s="6"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="6"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A14" s="6">
-        <v>5</v>
-      </c>
-      <c r="B14" s="6"/>
-      <c r="C14" s="6"/>
-      <c r="D14" s="6"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A15" s="6"/>
-      <c r="B15" s="6"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A16" s="6"/>
-      <c r="B16" s="6"/>
-      <c r="C16" s="6"/>
-      <c r="D16" s="6"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A17" s="6"/>
-      <c r="B17" s="6"/>
-      <c r="C17" s="6"/>
-      <c r="D17" s="6"/>
+      <c r="B11" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>42</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2068,11 +1710,11 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D01BD858-72F0-4803-BCED-49D604DC8C85}">
-  <dimension ref="A1:D17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6F2B678-6A08-4DCD-A7B0-10E20E2DA48D}">
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -2105,15 +1747,15 @@
         <v>1</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.15">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="15" x14ac:dyDescent="0.15">
       <c r="A6" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C6" s="2"/>
     </row>
@@ -2122,7 +1764,7 @@
         <v>4</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -2142,63 +1784,61 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A10" s="6">
-        <v>1</v>
-      </c>
-      <c r="B10" s="6"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A11" s="6">
+    <row r="10" spans="1:4" ht="30" x14ac:dyDescent="0.15">
+      <c r="A10" s="7">
+        <v>1</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.15">
+      <c r="A11" s="7">
         <v>2</v>
       </c>
-      <c r="B11" s="6"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A12" s="6">
+      <c r="B11" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.15">
+      <c r="A12" s="7">
         <v>3</v>
       </c>
-      <c r="B12" s="6"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A13" s="6">
+      <c r="B12" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.15">
+      <c r="A13" s="7">
         <v>4</v>
       </c>
-      <c r="B13" s="6"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="6"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A14" s="6">
-        <v>5</v>
-      </c>
-      <c r="B14" s="6"/>
-      <c r="C14" s="6"/>
-      <c r="D14" s="6"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A15" s="6"/>
-      <c r="B15" s="6"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A16" s="6"/>
-      <c r="B16" s="6"/>
-      <c r="C16" s="6"/>
-      <c r="D16" s="6"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A17" s="6"/>
-      <c r="B17" s="6"/>
-      <c r="C17" s="6"/>
-      <c r="D17" s="6"/>
+      <c r="B13" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>40</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>